<commit_message>
labreport 5 & tokdebate
</commit_message>
<xml_diff>
--- a/whk/whklatex/physics/5/data/Book1.xlsx
+++ b/whk/whklatex/physics/5/data/Book1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\whk\whklatex\physics\5\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538A2DE0-A0A2-418D-9311-C7230F1FCE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAB5C4C-7FDC-47E6-ABDF-87863FB2B758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="17280" windowHeight="10043" xr2:uid="{D54FC7CC-7B09-44DB-8C63-ABDEA91A66AB}"/>
+    <workbookView xWindow="1522" yWindow="2467" windowWidth="21600" windowHeight="11296" xr2:uid="{D54FC7CC-7B09-44DB-8C63-ABDEA91A66AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>n</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,23 +45,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Delta T Range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Experiment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>l(cm)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Start(s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>End (s)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -71,11 +56,47 @@
     <t>Period(s)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Error T(s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage Error T(s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t0(s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 (s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T^2(s^2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg. Period</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error T^2(s^2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.000_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,14 +136,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -439,44 +463,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E245B8-B25F-4C9C-B349-BD3845D6EC25}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
         <v>10</v>
       </c>
@@ -496,16 +538,35 @@
         <f>E2-D2</f>
         <v>13.799999999999999</v>
       </c>
-      <c r="H2">
-        <f>G2/F2/2</f>
-        <v>0.17249999999999999</v>
-      </c>
-      <c r="I2">
-        <f>MAX(G2:G6)-MIN(G2:G6)</f>
-        <v>0.39999999999999858</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H2" s="2">
+        <f>G2/(F2/2)</f>
+        <v>0.69</v>
+      </c>
+      <c r="I2" s="2">
+        <f>AVERAGE(H2:H6)</f>
+        <v>0.67799999999999994</v>
+      </c>
+      <c r="J2" s="2">
+        <f>(MAX(G2:G6)-MIN(G2:G6))/2</f>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="K2" s="1">
+        <f>J2/G2</f>
+        <v>1.4492753623188356E-2</v>
+      </c>
+      <c r="L2" s="2">
+        <f>I2*I2</f>
+        <v>0.45968399999999993</v>
+      </c>
+      <c r="M2" s="2">
+        <f>2*K2*L2</f>
+        <v>1.3324173913043431E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3">
         <v>10</v>
       </c>
@@ -525,12 +586,20 @@
         <f t="shared" ref="G3:G26" si="0">E3-D3</f>
         <v>13.4</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H26" si="1">G3/F3/2</f>
-        <v>0.16750000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H26" si="1">G3/(F3/2)</f>
+        <v>0.67</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
       <c r="B4">
         <v>10</v>
       </c>
@@ -550,12 +619,20 @@
         <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>0.16875000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="B5">
         <v>10</v>
       </c>
@@ -575,12 +652,20 @@
         <f t="shared" si="0"/>
         <v>13.6</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>0.16999999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
       <c r="B6">
         <v>10</v>
       </c>
@@ -600,12 +685,20 @@
         <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>0.16875000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
       <c r="B7">
         <v>20</v>
       </c>
@@ -625,16 +718,35 @@
         <f t="shared" si="0"/>
         <v>19.099999999999998</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>0.23874999999999996</v>
-      </c>
-      <c r="I7">
-        <f>MAX(G7:G11)-MIN(G7:G11)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.95499999999999985</v>
+      </c>
+      <c r="I7" s="2">
+        <f>AVERAGE(H7:H11)</f>
+        <v>0.95300000000000007</v>
+      </c>
+      <c r="J7" s="2">
+        <f>(MAX(G7:G11)-MIN(G7:G11))/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="K7" s="1">
+        <f>J7/G7</f>
+        <v>1.3089005235602096E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <f>I7*I7</f>
+        <v>0.90820900000000016</v>
+      </c>
+      <c r="M7" s="2">
+        <f>2*K7*L7</f>
+        <v>2.3775104712041892E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
       <c r="B8">
         <v>20</v>
       </c>
@@ -654,12 +766,20 @@
         <f t="shared" si="0"/>
         <v>18.8</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>0.23500000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
       <c r="B9">
         <v>20</v>
       </c>
@@ -679,12 +799,20 @@
         <f t="shared" si="0"/>
         <v>19.200000000000003</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>0.24000000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.96000000000000019</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
       <c r="B10">
         <v>20</v>
       </c>
@@ -704,12 +832,20 @@
         <f t="shared" si="0"/>
         <v>19.3</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>0.24125000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
       <c r="B11">
         <v>20</v>
       </c>
@@ -729,12 +865,20 @@
         <f t="shared" si="0"/>
         <v>18.899999999999999</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>0.23624999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3</v>
+      </c>
       <c r="B12">
         <v>30</v>
       </c>
@@ -754,16 +898,35 @@
         <f t="shared" si="0"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>0.28500000000000003</v>
-      </c>
-      <c r="I12">
-        <f>MAX(G12:G16)-MIN(G12:G16)</f>
-        <v>0.30000000000000426</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="I12" s="2">
+        <f>AVERAGE(H12:H16)</f>
+        <v>1.1413333333333333</v>
+      </c>
+      <c r="J12" s="2">
+        <f>(MAX(G12:G16)-MIN(G12:G16))/2</f>
+        <v>0.15000000000000213</v>
+      </c>
+      <c r="K12" s="1">
+        <f>J12/G12</f>
+        <v>8.7719298245615279E-3</v>
+      </c>
+      <c r="L12" s="2">
+        <f>I12*I12</f>
+        <v>1.3026417777777777</v>
+      </c>
+      <c r="M12" s="2">
+        <f>2*K12*L12</f>
+        <v>2.2853364522417475E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
       <c r="B13">
         <v>30</v>
       </c>
@@ -783,12 +946,20 @@
         <f t="shared" si="0"/>
         <v>17.300000000000004</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>0.28833333333333339</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1533333333333335</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3</v>
+      </c>
       <c r="B14">
         <v>30</v>
       </c>
@@ -808,12 +979,20 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>0.28333333333333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1333333333333333</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3</v>
+      </c>
       <c r="B15">
         <v>30</v>
       </c>
@@ -833,12 +1012,20 @@
         <f t="shared" si="0"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>0.28500000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
       <c r="B16">
         <v>30</v>
       </c>
@@ -858,12 +1045,20 @@
         <f t="shared" si="0"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
-        <v>0.28500000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4</v>
+      </c>
       <c r="B17">
         <v>40</v>
       </c>
@@ -883,16 +1078,35 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="I17">
-        <f>MAX(G17:G21)-MIN(G17:G21)</f>
-        <v>0.1000000000000032</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="I17" s="2">
+        <f>AVERAGE(H17:H21)</f>
+        <v>1.304</v>
+      </c>
+      <c r="J17" s="2">
+        <f>(MAX(G17:G21)-MIN(G17:G21))/2</f>
+        <v>5.0000000000001599E-2</v>
+      </c>
+      <c r="K17" s="1">
+        <f>J17/G17</f>
+        <v>3.8461538461539691E-3</v>
+      </c>
+      <c r="L17" s="2">
+        <f>I17*I17</f>
+        <v>1.7004160000000001</v>
+      </c>
+      <c r="M17" s="2">
+        <f>2*K17*L17</f>
+        <v>1.3080123076923496E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
       <c r="B18">
         <v>40</v>
       </c>
@@ -912,12 +1126,20 @@
         <f t="shared" si="0"/>
         <v>13.1</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
-        <v>0.32750000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.31</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
       <c r="B19">
         <v>40</v>
       </c>
@@ -937,12 +1159,20 @@
         <f t="shared" si="0"/>
         <v>13.100000000000001</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
-        <v>0.32750000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>1.31</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4</v>
+      </c>
       <c r="B20">
         <v>40</v>
       </c>
@@ -962,12 +1192,20 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
-        <v>0.32500000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>4</v>
+      </c>
       <c r="B21">
         <v>40</v>
       </c>
@@ -987,138 +1225,330 @@
         <f t="shared" si="0"/>
         <v>12.999999999999998</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="1"/>
-        <v>0.32499999999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>5</v>
+      </c>
       <c r="B22">
         <v>50</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
         <v>3.8</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22">
         <v>17.3</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22">
         <v>19</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
-        <v>0.35526315789473684</v>
-      </c>
-      <c r="I22">
-        <f>MAX(G22:G26)-MIN(G22:G26)</f>
-        <v>1.0000000000000071</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4210526315789473</v>
+      </c>
+      <c r="I22" s="2">
+        <f>AVERAGE(H22:H26)</f>
+        <v>1.4463157894736842</v>
+      </c>
+      <c r="J22" s="2">
+        <f>(MAX(G22:G26)-MIN(G22:G26))/2</f>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="K22" s="1">
+        <f>J22/G22</f>
+        <v>1.4814814814814828E-2</v>
+      </c>
+      <c r="L22" s="2">
+        <f>I22*I22</f>
+        <v>2.0918293628808864</v>
+      </c>
+      <c r="M22" s="2">
+        <f>2*K22*L22</f>
+        <v>6.1980129270544838E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>5</v>
+      </c>
       <c r="B23">
         <v>50</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="2">
-        <v>57.9</v>
-      </c>
-      <c r="E23" s="2">
-        <v>72.400000000000006</v>
-      </c>
-      <c r="F23" s="1">
+      <c r="D23">
+        <v>59.4</v>
+      </c>
+      <c r="E23">
+        <v>73.2</v>
+      </c>
+      <c r="F23">
         <v>19</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>14.500000000000007</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
-        <v>0.38157894736842124</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+        <v>13.800000000000004</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4526315789473689</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
       <c r="B24">
         <v>50</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24">
         <v>28.8</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24">
         <v>42.5</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24">
         <v>19</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
         <v>13.7</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="1"/>
-        <v>0.36052631578947364</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4421052631578946</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>5</v>
+      </c>
       <c r="B25">
         <v>50</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25">
         <v>18.399999999999999</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25">
         <v>32.200000000000003</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25">
         <v>19</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
         <v>13.800000000000004</v>
       </c>
-      <c r="H25">
-        <f t="shared" si="1"/>
-        <v>0.36315789473684223</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4526315789473689</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5</v>
+      </c>
       <c r="B26">
         <v>50</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26">
         <v>13.9</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>27.8</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26">
         <v>19</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
         <v>13.9</v>
       </c>
-      <c r="H26">
-        <f t="shared" si="1"/>
-        <v>0.36578947368421055</v>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4631578947368422</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5043FE73-B2A3-4B2C-BD78-B39E5C446300}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.67799999999999994</v>
+      </c>
+      <c r="C2">
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.4492753623188356E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.45968399999999993</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.3324173913043431E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.95300000000000007</v>
+      </c>
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.3089005235602096E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.90820900000000016</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2.3775104712041892E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.1413333333333333</v>
+      </c>
+      <c r="C4">
+        <v>0.15000000000000213</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.7719298245615279E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.3026417777777777</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2.2853364522417475E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.304</v>
+      </c>
+      <c r="C5">
+        <v>5.0000000000001599E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3.8461538461539691E-3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.7004160000000001</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.3080123076923496E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.4463157894736842</v>
+      </c>
+      <c r="C6">
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.4814814814814828E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.0918293628808864</v>
+      </c>
+      <c r="F6" s="3">
+        <v>6.1980129270544838E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>